<commit_message>
Implement IgnoreTrailingEmptyRows for xls
</commit_message>
<xml_diff>
--- a/source/Sylvan.Data.Excel.Tests/Data/TrailingBlank.xlsx
+++ b/source/Sylvan.Data.Excel.Tests/Data/TrailingBlank.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\source\Sylvan.Data.Excel\source\Sylvan.Data.Excel.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E52485-F8A1-4C03-82E3-B0E4B2F545F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{21E655EA-42D9-4670-8A5B-68F8B3388B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="840" windowWidth="27960" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="840" windowWidth="27960" windowHeight="13776"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -39,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,20 +336,15 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,6 +376,36 @@
         <v/>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>